<commit_message>
accelpressure done. work on making figure
</commit_message>
<xml_diff>
--- a/Power/Cut10000.xlsx
+++ b/Power/Cut10000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>14.30727481842041</v>
+        <v>8594.505859375</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1698.399047851562</v>
+        <v>1900.897094726562</v>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>2.222222222222222</v>
@@ -485,884 +485,940 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2472.776123046875</v>
+        <v>1653.625610351562</v>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>1.052631578947368</v>
+        <v>2.857142857142857</v>
       </c>
       <c r="D4" t="n">
-        <v>3.27485380116959</v>
+        <v>5.079365079365079</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5118.47900390625</v>
+        <v>1653.625610351562</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1.481481481481482</v>
+        <v>4.444444444444445</v>
       </c>
       <c r="D5" t="n">
-        <v>4.756335282651072</v>
+        <v>9.523809523809524</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5936.61181640625</v>
+        <v>4524.21337890625</v>
       </c>
       <c r="B6" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5882352941176467</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>5.344570576768719</v>
+        <v>12.85714285714286</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7239.11181640625</v>
+        <v>8478.298828125</v>
       </c>
       <c r="B7" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5263157894736841</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>5.870886366242403</v>
+        <v>14.85714285714286</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7711.26806640625</v>
+        <v>18554.083984375</v>
       </c>
       <c r="B8" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>1.363636363636363</v>
+        <v>3.75</v>
       </c>
       <c r="D8" t="n">
-        <v>7.234522729878766</v>
+        <v>18.60714285714286</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7943.27587890625</v>
+        <v>41376.64453125</v>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7999999999999998</v>
+        <v>5.185185185185185</v>
       </c>
       <c r="D9" t="n">
-        <v>8.034522729878766</v>
+        <v>23.79232804232804</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>11484.4482421875</v>
+        <v>50227.77734375</v>
       </c>
       <c r="B10" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>3.606557377049183</v>
+        <v>2.162162162162162</v>
       </c>
       <c r="D10" t="n">
-        <v>11.64108010692795</v>
+        <v>25.95449020449021</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10328.4794921875</v>
+        <v>50799.57421875</v>
       </c>
       <c r="B11" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>1.19402985074626</v>
+        <v>0.975609756097561</v>
       </c>
       <c r="D11" t="n">
-        <v>12.83510995767421</v>
+        <v>26.93009996058777</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7430.41650390625</v>
+        <v>24190.767578125</v>
       </c>
       <c r="B12" t="n">
-        <v>24.04334817728194</v>
+        <v>18</v>
       </c>
       <c r="C12" t="n">
-        <v>2.942797502087171</v>
+        <v>2.051282051282051</v>
       </c>
       <c r="D12" t="n">
-        <v>15.77790745976138</v>
+        <v>28.98138201186982</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>57631.71484375</v>
+        <v>4393.96337890625</v>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6891316742798601</v>
+        <v>6.108304630544683</v>
       </c>
       <c r="D13" t="n">
-        <v>16.46703913404124</v>
+        <v>35.0896866424145</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1787.945922851562</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>2.67077872256592</v>
+        <v>2.357022603955159</v>
       </c>
       <c r="D14" t="n">
-        <v>19.13781785660716</v>
+        <v>37.44670924636966</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>4039.846435546875</v>
+        <v>16694.365234375</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8695652173913082</v>
+        <v>6.009252125773315</v>
       </c>
       <c r="D15" t="n">
-        <v>20.00738307399847</v>
+        <v>43.45596137214297</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4532.35400390625</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B16" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>1.490711984999852</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="D16" t="n">
-        <v>21.49809505899832</v>
+        <v>45.27414319032479</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8154.93212890625</v>
+        <v>2511.444091796875</v>
       </c>
       <c r="B17" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>2.693740118805898</v>
+        <v>8.944271909999159</v>
       </c>
       <c r="D17" t="n">
-        <v>24.19183517780422</v>
+        <v>54.21841510032395</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3893.315185546875</v>
+        <v>22004.236328125</v>
       </c>
       <c r="B18" t="n">
-        <v>20.33829352893933</v>
+        <v>11</v>
       </c>
       <c r="C18" t="n">
-        <v>4.34460895424289</v>
+        <v>8.081220356417687</v>
       </c>
       <c r="D18" t="n">
-        <v>28.53644413204711</v>
+        <v>62.29963545674164</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>6160.47900390625</v>
+        <v>8865.7099609375</v>
       </c>
       <c r="B19" t="n">
-        <v>23</v>
+        <v>10.63749142467192</v>
       </c>
       <c r="C19" t="n">
-        <v>1.305278493652491</v>
+        <v>9.103511685801108</v>
       </c>
       <c r="D19" t="n">
-        <v>29.8417226256996</v>
+        <v>71.40314714254275</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8944.5732421875</v>
+        <v>5179.53369140625</v>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9126808071427703</v>
+        <v>2.880639959127004</v>
       </c>
       <c r="D20" t="n">
-        <v>30.75440343284237</v>
+        <v>74.28378710166976</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>143572.0625</v>
+        <v>26740.583984375</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4347826086956594</v>
+        <v>2.1295885499998</v>
       </c>
       <c r="D21" t="n">
-        <v>31.18918604153803</v>
+        <v>76.41337565166955</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>6038.36962890625</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B22" t="n">
-        <v>25.01196482921286</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>3.796325611528268</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="D22" t="n">
-        <v>34.9855116530663</v>
+        <v>77.52448676278067</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>10067.9794921875</v>
+        <v>15735.3154296875</v>
       </c>
       <c r="B23" t="n">
-        <v>28</v>
+        <v>11.01196482921286</v>
       </c>
       <c r="C23" t="n">
-        <v>0.843608790847</v>
+        <v>10.04469951718429</v>
       </c>
       <c r="D23" t="n">
-        <v>35.8291204439133</v>
+        <v>87.56918627996497</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>9644.6669921875</v>
+        <v>34399.63671875</v>
       </c>
       <c r="B24" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7710579232757908</v>
+        <v>1.787998658056773</v>
       </c>
       <c r="D24" t="n">
-        <v>36.60017836718909</v>
+        <v>89.35718493802175</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>6913.48681640625</v>
+        <v>37390.48046875</v>
       </c>
       <c r="B25" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C25" t="n">
-        <v>1.856953381770509</v>
+        <v>1.49071198499986</v>
       </c>
       <c r="D25" t="n">
-        <v>38.4571317489596</v>
+        <v>90.84789692302161</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>239284.25</v>
+        <v>16321.2607421875</v>
       </c>
       <c r="B26" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4166666666666714</v>
+        <v>3.590109871423003</v>
       </c>
       <c r="D26" t="n">
-        <v>38.87379841562627</v>
+        <v>94.4380067944446</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>5948.82275390625</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B27" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>2.447802185061128</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>41.3216006006874</v>
+        <v>95.4380067944446</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>5692.39306640625</v>
+        <v>14554.37890625</v>
       </c>
       <c r="B28" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6017930052651508</v>
+        <v>6.73145600891813</v>
       </c>
       <c r="D28" t="n">
-        <v>41.92339360595255</v>
+        <v>102.1694628033627</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>4597.47900390625</v>
+        <v>5053.35400390625</v>
       </c>
       <c r="B29" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C29" t="n">
-        <v>1.963383631246515</v>
+        <v>1.488645855129574</v>
       </c>
       <c r="D29" t="n">
-        <v>43.88677723719906</v>
+        <v>103.6581086584923</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>7890.36181640625</v>
+        <v>2468.705810546875</v>
       </c>
       <c r="B30" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>0.5</v>
+        <v>5.890150893739516</v>
       </c>
       <c r="D30" t="n">
-        <v>44.38677723719906</v>
+        <v>109.5482595522318</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4967.87744140625</v>
+        <v>12573.4228515625</v>
       </c>
       <c r="B31" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C31" t="n">
-        <v>1.81818181818182</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="D31" t="n">
-        <v>46.20495905538088</v>
+        <v>111.2149262188985</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7780.46337890625</v>
+        <v>8779.3212890625</v>
       </c>
       <c r="B32" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C32" t="n">
-        <v>2.854945054619805</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="D32" t="n">
-        <v>49.05990411000069</v>
+        <v>112.5482595522318</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5545.86181640625</v>
+        <v>35344.87890625</v>
       </c>
       <c r="B33" t="n">
-        <v>27.90418795780726</v>
+        <v>16</v>
       </c>
       <c r="C33" t="n">
-        <v>2.399893166344633</v>
+        <v>8.158431221748456</v>
       </c>
       <c r="D33" t="n">
-        <v>51.45979727634532</v>
+        <v>120.7066907739803</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>11061.1357421875</v>
+        <v>6705.90087890625</v>
       </c>
       <c r="B34" t="n">
-        <v>35</v>
+        <v>11.66170647106067</v>
       </c>
       <c r="C34" t="n">
-        <v>3.273432334232737</v>
+        <v>5.829183211623753</v>
       </c>
       <c r="D34" t="n">
-        <v>54.73322961057806</v>
+        <v>126.535873985604</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>8309.6044921875</v>
+        <v>51982.15234375</v>
       </c>
       <c r="B35" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C35" t="n">
-        <v>3.16774400419677</v>
+        <v>5.649898825367719</v>
       </c>
       <c r="D35" t="n">
-        <v>57.90097361477483</v>
+        <v>132.1857728109718</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>69286.8125</v>
+        <v>31559.291015625</v>
       </c>
       <c r="B36" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C36" t="n">
-        <v>1.792654619833776</v>
+        <v>5.668594533825794</v>
       </c>
       <c r="D36" t="n">
-        <v>59.6936282346086</v>
+        <v>137.8543673447976</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4727.72900390625</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B37" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C37" t="n">
-        <v>0.9753196981883363</v>
+        <v>4.123105625617661</v>
       </c>
       <c r="D37" t="n">
-        <v>60.66894793279694</v>
+        <v>141.9774729704152</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>6494.24462890625</v>
+        <v>1644.467407226562</v>
       </c>
       <c r="B38" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>1.242259987499878</v>
+        <v>7.071067811865476</v>
       </c>
       <c r="D38" t="n">
-        <v>61.91120792029682</v>
+        <v>149.0485407822807</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>5541.79150390625</v>
+        <v>5199.88525390625</v>
       </c>
       <c r="B39" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C39" t="n">
-        <v>3.214121732666129</v>
+        <v>7.905694150420948</v>
       </c>
       <c r="D39" t="n">
-        <v>65.12532965296295</v>
+        <v>156.9542349327016</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>10922.7451171875</v>
+        <v>11461.6923828125</v>
       </c>
       <c r="B40" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C40" t="n">
-        <v>2.181818181818187</v>
+        <v>4</v>
       </c>
       <c r="D40" t="n">
-        <v>67.30714783478113</v>
+        <v>160.9542349327016</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>14801.32421875</v>
+        <v>36721.51171875</v>
       </c>
       <c r="B41" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C41" t="n">
-        <v>1.492537313432834</v>
+        <v>7.244308110509934</v>
       </c>
       <c r="D41" t="n">
-        <v>68.79968514821397</v>
+        <v>168.1985430432116</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>264946.90625</v>
+        <v>63091.8984375</v>
       </c>
       <c r="B42" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C42" t="n">
-        <v>0.7985957062499267</v>
+        <v>2.702702702702703</v>
       </c>
       <c r="D42" t="n">
-        <v>69.59828085446389</v>
+        <v>170.9012457459143</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>6156.40869140625</v>
+        <v>14.30727481842041</v>
       </c>
       <c r="B43" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>1.49071198499986</v>
+        <v>1.720052290384454</v>
       </c>
       <c r="D43" t="n">
-        <v>71.08899283946376</v>
+        <v>172.6212980362987</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5037.07275390625</v>
+        <v>8538.3310546875</v>
       </c>
       <c r="B44" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C44" t="n">
-        <v>2.142857142857143</v>
+        <v>2.357022603955159</v>
       </c>
       <c r="D44" t="n">
-        <v>73.2318499823209</v>
+        <v>174.9783206402539</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>6844.29150390625</v>
+        <v>437.1109924316406</v>
       </c>
       <c r="B45" t="n">
-        <v>19</v>
+        <v>1.917078252831711</v>
       </c>
       <c r="C45" t="n">
-        <v>0.5555555555555556</v>
+        <v>9.247660519987756</v>
       </c>
       <c r="D45" t="n">
-        <v>73.78740553787645</v>
+        <v>184.2259811602416</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3775.276123046875</v>
+        <v>4695.16650390625</v>
       </c>
       <c r="B46" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>2.692582403567252</v>
+        <v>3.380046561058861</v>
       </c>
       <c r="D46" t="n">
-        <v>76.47998794144371</v>
+        <v>187.6060277213005</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>7198.40869140625</v>
+        <v>4247.43212890625</v>
       </c>
       <c r="B47" t="n">
-        <v>26</v>
+        <v>5.338293528939332</v>
       </c>
       <c r="C47" t="n">
-        <v>2.724733718056531</v>
+        <v>4.789029110233523</v>
       </c>
       <c r="D47" t="n">
-        <v>79.20472165950024</v>
+        <v>192.395056831534</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5244.65869140625</v>
+        <v>16421.029296875</v>
       </c>
       <c r="B48" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C48" t="n">
-        <v>2.37998036524298</v>
+        <v>10.53026162347456</v>
       </c>
       <c r="D48" t="n">
-        <v>81.58470202474322</v>
+        <v>202.9253184550086</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>4719.58837890625</v>
+        <v>21095.669921875</v>
       </c>
       <c r="B49" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C49" t="n">
-        <v>1.754513032177728</v>
+        <v>1.229750923802691</v>
       </c>
       <c r="D49" t="n">
-        <v>83.33921505692095</v>
+        <v>204.1550693788113</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>9025.9794921875</v>
+        <v>6351.78369140625</v>
       </c>
       <c r="B50" t="n">
-        <v>31</v>
+        <v>10.8799729114185</v>
       </c>
       <c r="C50" t="n">
-        <v>4.016494915340822</v>
+        <v>1.954607189577446</v>
       </c>
       <c r="D50" t="n">
-        <v>87.35570997226178</v>
+        <v>206.1096765683887</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>11272.7919921875</v>
+        <v>18366.142578125</v>
       </c>
       <c r="B51" t="n">
-        <v>32</v>
+        <v>12.78491521734411</v>
       </c>
       <c r="C51" t="n">
-        <v>0.3174603174603174</v>
+        <v>8.823457311189456</v>
       </c>
       <c r="D51" t="n">
-        <v>87.67317028972209</v>
+        <v>214.9331338795782</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>7230.97119140625</v>
+        <v>36686.33984375</v>
       </c>
       <c r="B52" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C52" t="n">
-        <v>2.903225806451613</v>
+        <v>5.413651635042291</v>
       </c>
       <c r="D52" t="n">
-        <v>90.57639609617371</v>
+        <v>220.3467855146205</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>7751.97119140625</v>
+        <v>50221.10546875</v>
       </c>
       <c r="B53" t="n">
-        <v>31.20338585353982</v>
+        <v>19</v>
       </c>
       <c r="C53" t="n">
-        <v>1.666254061758863</v>
+        <v>1.111111111111111</v>
       </c>
       <c r="D53" t="n">
-        <v>92.24265015793257</v>
+        <v>221.4578966257316</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>6852.43212890625</v>
+        <v>54190.05859375</v>
       </c>
       <c r="B54" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C54" t="n">
-        <v>3.280779019725987</v>
+        <v>0.5128205128205128</v>
       </c>
       <c r="D54" t="n">
-        <v>95.52342917765856</v>
+        <v>221.9707171385521</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>5089.98681640625</v>
+        <v>61460.26171875</v>
       </c>
       <c r="B55" t="n">
-        <v>23.54124236468912</v>
+        <v>22</v>
       </c>
       <c r="C55" t="n">
-        <v>1.48556200864229</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="D55" t="n">
-        <v>97.00899118630085</v>
+        <v>222.9230980909331</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>3901.455810546875</v>
+        <v>37622.54296875</v>
       </c>
       <c r="B56" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C56" t="n">
-        <v>2.148631942749128</v>
+        <v>4.285714285714286</v>
       </c>
       <c r="D56" t="n">
-        <v>99.15762312904998</v>
+        <v>227.2088123766474</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>8684.0732421875</v>
+        <v>5777.86962890625</v>
       </c>
       <c r="B57" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C57" t="n">
-        <v>2.111829336131178</v>
+        <v>6.735681618651967</v>
       </c>
       <c r="D57" t="n">
-        <v>101.2694524651812</v>
+        <v>233.9444939952993</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>10418.0263671875</v>
+        <v>5692.39306640625</v>
       </c>
       <c r="B58" t="n">
-        <v>31</v>
+        <v>9.541242364689118</v>
       </c>
       <c r="C58" t="n">
-        <v>1.071958528870637</v>
+        <v>3.51054839960607</v>
       </c>
       <c r="D58" t="n">
-        <v>102.3414109940518</v>
+        <v>237.4550423949054</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>6771.02587890625</v>
+        <v>5737.16650390625</v>
       </c>
       <c r="B59" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C59" t="n">
-        <v>2.968978733815546</v>
+        <v>5.393381847510125</v>
       </c>
       <c r="D59" t="n">
-        <v>105.3103897278673</v>
+        <v>242.8484242424155</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8749.1982421875</v>
+        <v>30094.345703125</v>
       </c>
       <c r="B60" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C60" t="n">
-        <v>1.612903225806452</v>
+        <v>4.682752006203916</v>
       </c>
       <c r="D60" t="n">
-        <v>106.9232929536738</v>
+        <v>247.5311762486194</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>9074.8232421875</v>
+        <v>25535.259765625</v>
       </c>
       <c r="B61" t="n">
-        <v>28.6003046877419</v>
+        <v>15</v>
       </c>
       <c r="C61" t="n">
-        <v>1.360754090878911</v>
+        <v>4.876598490941707</v>
       </c>
       <c r="D61" t="n">
-        <v>108.2840470445527</v>
+        <v>252.4077747395611</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>3647.061279296875</v>
+        <v>39161.56640625</v>
       </c>
       <c r="B62" t="n">
-        <v>20.29658149148228</v>
+        <v>16</v>
       </c>
       <c r="C62" t="n">
-        <v>9.825093651519612</v>
+        <v>0.6451612903225806</v>
       </c>
       <c r="D62" t="n">
-        <v>118.1091406960723</v>
+        <v>253.0529360298837</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>8089.80712890625</v>
+        <v>46474.91015625</v>
       </c>
       <c r="B63" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C63" t="n">
-        <v>3.078493057935532</v>
+        <v>1.176470588235294</v>
       </c>
       <c r="D63" t="n">
-        <v>121.1876337540078</v>
+        <v>254.229406618119</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>7145.49462890625</v>
+        <v>53975.96484375</v>
       </c>
       <c r="B64" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>2.172415189392221</v>
+        <v>1.052631578947368</v>
       </c>
       <c r="D64" t="n">
-        <v>123.3600489434001</v>
+        <v>255.2820381970664</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>5851.13525390625</v>
+        <v>65647.4609375</v>
       </c>
       <c r="B65" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C65" t="n">
-        <v>3.482840437745161</v>
+        <v>4</v>
       </c>
       <c r="D65" t="n">
-        <v>126.8428893811452</v>
+        <v>259.2820381970664</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>5733.09619140625</v>
+        <v>12452.5263671875</v>
       </c>
       <c r="B66" t="n">
-        <v>20.62096934546506</v>
+        <v>13</v>
       </c>
       <c r="C66" t="n">
-        <v>1.025226174957644</v>
+        <v>11.57894736842105</v>
       </c>
       <c r="D66" t="n">
-        <v>127.8681155561029</v>
+        <v>270.8609855654875</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>12876.4794921875</v>
+      </c>
+      <c r="B67" t="n">
+        <v>12.43989448617086</v>
+      </c>
+      <c r="C67" t="n">
+        <v>2.4860776540464</v>
+      </c>
+      <c r="D67" t="n">
+        <v>273.3470632195339</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>27978.830078125</v>
+      </c>
+      <c r="B68" t="n">
+        <v>15</v>
+      </c>
+      <c r="C68" t="n">
+        <v>5.153859330930844</v>
+      </c>
+      <c r="D68" t="n">
+        <v>278.5009225504647</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>43222.87109375</v>
+      </c>
+      <c r="B69" t="n">
+        <v>18</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2.424242424242424</v>
+      </c>
+      <c r="D69" t="n">
+        <v>280.9251649747072</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>6596.00244140625</v>
+      </c>
+      <c r="B70" t="n">
+        <v>12</v>
+      </c>
+      <c r="C70" t="n">
+        <v>5.497474167490214</v>
+      </c>
+      <c r="D70" t="n">
+        <v>286.4226391421974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>